<commit_message>
missing reference in last question
</commit_message>
<xml_diff>
--- a/bluevector/question-answer.xlsx
+++ b/bluevector/question-answer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericliang/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD62C542-A996-FA40-8679-E5F9DA67B1A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C327A89E-45DE-4045-BF54-E0D223461182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19440" xr2:uid="{9CE88A78-9CD4-8D43-967D-9F0BDFC5B8A7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
   <si>
     <t>question</t>
   </si>
@@ -667,7 +667,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -809,12 +809,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B13" t="s">
         <v>27</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>